<commit_message>
finalized single exp excel
</commit_message>
<xml_diff>
--- a/Templates/Generic_single.xlsx
+++ b/Templates/Generic_single.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laghi\Documents\03_dottorato\04_F4E\01_JADE\Code\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE554D56-DEF8-4131-A6B4-C11975582FD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7F5DCF-A2C9-4270-B876-7C844BF406E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E67D81CA-4E2B-403F-A5FA-739B76A12615}"/>
+    <workbookView xWindow="33150" yWindow="660" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{E67D81CA-4E2B-403F-A5FA-739B76A12615}"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="3" r:id="rId1"/>
     <sheet name="Errors" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,9 +34,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>LIBRARY:</t>
+  </si>
+  <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>&gt; 50%</t>
+  </si>
+  <si>
+    <t>20% ≤ 50 %</t>
+  </si>
+  <si>
+    <t>10% ≤ 20 %</t>
+  </si>
+  <si>
+    <t>&lt; 10%</t>
+  </si>
+  <si>
+    <t>according to MCNP manual</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,16 +78,104 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -66,11 +183,297 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -78,11 +481,250 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valore valido" xfId="1" builtinId="26"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -106,6 +748,27 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Values"/>
+      <sheetName val="Errors"/>
+      <sheetName val="Statistical Checks"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="C1"/>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,10 +1068,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FDEA1D-8E37-426E-874F-F31ECF16F597}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N7:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -416,9 +1080,123 @@
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="2"/>
   </cols>
-  <sheetData/>
-  <conditionalFormatting sqref="B1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <sheetData>
+    <row r="1" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="16">
+        <f>[1]Values!C1</f>
+        <v>0</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="A3:K7"/>
+  </mergeCells>
+  <conditionalFormatting sqref="O1:XFD2 B8:L1048576 M3:XFD1048576">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"total"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -429,10 +1207,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957049AC-9C45-4A72-BB36-9A6B1DE33BC9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,10 +1219,281 @@
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="2"/>
   </cols>
-  <sheetData/>
-  <conditionalFormatting sqref="B1:XFD1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <sheetData>
+    <row r="1" spans="1:22" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="33">
+        <f>[1]Values!C1</f>
+        <v>0</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:22" ht="21.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+    </row>
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="46"/>
+      <c r="O3" s="47"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="49"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="49"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="39"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="49"/>
+    </row>
+    <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="51"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="11"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="11"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="11"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="11"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="11"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="11"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="11"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="11"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="C14:V14"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="A3:K7"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="M2:O2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B8:XFD10 B40:XFD1048576 W11:XFD39 P1:XFD7">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"total"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"total"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:V13 B15:V39 B14:C14">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"total"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:AAA1048576">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
+      <formula>1E-30</formula>
+      <formula>0.1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+      <formula>0.1</formula>
+      <formula>0.2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+      <formula>0.2</formula>
+      <formula>0.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="between">
+      <formula>0.5</formula>
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>